<commit_message>
Multa fija agua externa
</commit_message>
<xml_diff>
--- a/parametros_reales.xlsx
+++ b/parametros_reales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nacho/Folders/Ingenieria/Optimización/Gurobi-Opti/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB7FD7C-F66C-2342-909B-1BBDFFB43C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D5B4BE-CDA4-CC4B-9075-1DC7AD675727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4980" yWindow="1760" windowWidth="19580" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Parámetro</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>Volumen inicial del embalse (m³)</t>
-  </si>
-  <si>
-    <t>Costo agua externa (US$/m³)</t>
   </si>
   <si>
     <t>Presupuesto diario agua externa (US$/día)</t>
@@ -180,6 +177,15 @@
   </si>
   <si>
     <t>Multa fija por exceso (US$)</t>
+  </si>
+  <si>
+    <t>Pf</t>
+  </si>
+  <si>
+    <t>Costo de bombear agua externa (US$/m³)</t>
+  </si>
+  <si>
+    <t>Costo fijo de uso de agua externa (US$)</t>
   </si>
 </sst>
 </file>
@@ -550,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -634,7 +640,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C7">
         <v>5.45</v>
@@ -642,36 +648,36 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C8">
-        <v>1500000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9">
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
         <f>110 * 365</f>
         <v>40150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10">
-        <v>27000</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -679,31 +685,42 @@
         <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11">
-        <v>1000000</v>
+        <v>27000</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C12">
-        <v>25000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13">
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
         <v>1000000</v>
       </c>
     </row>
@@ -737,37 +754,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -863,25 +880,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -951,13 +968,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
cambio c por b
</commit_message>
<xml_diff>
--- a/parametros_reales.xlsx
+++ b/parametros_reales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/carlos_raineri_uc_cl/Documents/semestre 6/opti/PROYECTO/Gurobi-Opti/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{88D5B4BE-CDA4-CC4B-9075-1DC7AD675727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFB878B9-D9EF-4604-A746-99F3EFEB7083}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{88D5B4BE-CDA4-CC4B-9075-1DC7AD675727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD5D41CE-0D34-45F9-91C7-18C5FAD61FA3}"/>
   <bookViews>
     <workbookView xWindow="2328" yWindow="3024" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,7 +191,7 @@
     <t>beneficio recicular agua</t>
   </si>
   <si>
-    <t>C</t>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="136" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>